<commit_message>
changed icon and form titles
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/res/sokhnaColorReport.xlsx
+++ b/WatanyaPingTester/bin/Debug/res/sokhnaColorReport.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Fahim\C#\New folder\Pingo\WatanyaPingTester\bin\Debug\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New folder\New folder\Pingo\WatanyaPingTester\bin\Debug\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6855" windowHeight="4335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="83">
   <si>
-    <t>From: 1526 To: 1530</t>
+    <t>From: 0854 To: 0904</t>
   </si>
   <si>
     <t>Degla:</t>
@@ -285,6 +285,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="178"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -642,7 +643,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="6" width="18.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added date to report
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/res/sokhnaColorReport.xlsx
+++ b/WatanyaPingTester/bin/Debug/res/sokhnaColorReport.xlsx
@@ -26,7 +26,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="83">
   <si>
-    <t>From: 1220 To: 1248</t>
+    <t>From: 21-01-2018 at 0801
+To: 21-01-2018 at 0801</t>
   </si>
   <si>
     <t>Degla:</t>
@@ -339,13 +340,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -636,7 +640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -646,1888 +650,1892 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B5" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C5" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D5" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E5" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="F5" s="5">
-        <v>99.51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B11" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C11" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D11" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B17" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C17" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D17" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E17" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>0</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F22" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F23" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B23" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C23" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D23" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E23" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F23" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>0</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>0</v>
-      </c>
-      <c r="B27" s="5">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A30" s="4" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>0</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F33" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B33" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C33" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D33" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E33" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F33" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>0</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B37" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C37" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D37" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="40" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A40" s="4" t="s">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>0</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F42" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E43" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F43" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B43" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C43" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D43" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E43" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F43" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>0</v>
+      </c>
+      <c r="B44" s="6">
+        <v>0</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0</v>
+      </c>
+      <c r="E44" s="6">
+        <v>0</v>
+      </c>
+      <c r="F44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F46" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C47" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F47" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B47" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C47" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D47" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E47" s="5">
-        <v>0</v>
-      </c>
-      <c r="F47" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>0</v>
+      </c>
+      <c r="B48" s="6">
+        <v>0</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6">
+        <v>0</v>
+      </c>
+      <c r="E48" s="6">
+        <v>0</v>
+      </c>
+      <c r="F48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B50" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B51" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <v>0</v>
-      </c>
-      <c r="B51" s="5">
-        <v>0</v>
-      </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="54" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A54" s="4" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>0</v>
+      </c>
+      <c r="B52" s="6">
+        <v>0</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="55" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A55" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C56" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D56" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E56" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F56" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B57" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C57" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D57" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E57" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F57" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B57" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C57" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D57" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E57" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F57" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>0</v>
+      </c>
+      <c r="B58" s="6">
+        <v>0</v>
+      </c>
+      <c r="C58" s="6">
+        <v>0</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+      <c r="F58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C60" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D60" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E60" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F60" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B61" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C61" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D61" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E61" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F61" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B61" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C61" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D61" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E61" s="5">
-        <v>0</v>
-      </c>
-      <c r="F61" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>0</v>
+      </c>
+      <c r="B62" s="6">
+        <v>0</v>
+      </c>
+      <c r="C62" s="6">
+        <v>0</v>
+      </c>
+      <c r="D62" s="6">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0</v>
+      </c>
+      <c r="F62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B64" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B65" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
-        <v>0</v>
-      </c>
-      <c r="B65" s="5">
-        <v>0</v>
-      </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="68" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A68" s="4" t="s">
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>0</v>
+      </c>
+      <c r="B66" s="6">
+        <v>0</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="69" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A69" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B68" s="4"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B70" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C70" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D70" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E70" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F70" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B71" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C71" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D71" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E71" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F71" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B71" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C71" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D71" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E71" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F71" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>0</v>
+      </c>
+      <c r="B72" s="6">
+        <v>0</v>
+      </c>
+      <c r="C72" s="6">
+        <v>0</v>
+      </c>
+      <c r="D72" s="6">
+        <v>0</v>
+      </c>
+      <c r="E72" s="6">
+        <v>0</v>
+      </c>
+      <c r="F72" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D74" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E74" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F74" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B75" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C75" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D75" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E75" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F75" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B75" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C75" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D75" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E75" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F75" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>0</v>
+      </c>
+      <c r="B76" s="6">
+        <v>0</v>
+      </c>
+      <c r="C76" s="6">
+        <v>0</v>
+      </c>
+      <c r="D76" s="6">
+        <v>0</v>
+      </c>
+      <c r="E76" s="6">
+        <v>0</v>
+      </c>
+      <c r="F76" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B78" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D78" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B79" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C79" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D79" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B79" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="C79" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="D79" s="5">
-        <v>0</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-    </row>
-    <row r="82" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A82" s="4" t="s">
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>0</v>
+      </c>
+      <c r="B80" s="6">
+        <v>0</v>
+      </c>
+      <c r="C80" s="6">
+        <v>0</v>
+      </c>
+      <c r="D80" s="6">
+        <v>0</v>
+      </c>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="83" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A83" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B82" s="4"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B84" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C84" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D84" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E84" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F84" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B85" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C85" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E85" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F85" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B85" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C85" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D85" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E85" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F85" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>0</v>
+      </c>
+      <c r="B86" s="6">
+        <v>0</v>
+      </c>
+      <c r="C86" s="6">
+        <v>0</v>
+      </c>
+      <c r="D86" s="6">
+        <v>0</v>
+      </c>
+      <c r="E86" s="6">
+        <v>0</v>
+      </c>
+      <c r="F86" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B88" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C88" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D88" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E88" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F88" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B89" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C89" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D89" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E89" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F89" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B89" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C89" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D89" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E89" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F89" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>0</v>
+      </c>
+      <c r="B90" s="6">
+        <v>0</v>
+      </c>
+      <c r="C90" s="6">
+        <v>0</v>
+      </c>
+      <c r="D90" s="6">
+        <v>0</v>
+      </c>
+      <c r="E90" s="6">
+        <v>0</v>
+      </c>
+      <c r="F90" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B92" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C92" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D92" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E92" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F92" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B93" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C93" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D93" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E93" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F93" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B93" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="C93" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="D93" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E93" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F93" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>0</v>
+      </c>
+      <c r="B94" s="6">
+        <v>0</v>
+      </c>
+      <c r="C94" s="6">
+        <v>0</v>
+      </c>
+      <c r="D94" s="6">
+        <v>0</v>
+      </c>
+      <c r="E94" s="6">
+        <v>0</v>
+      </c>
+      <c r="F94" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B96" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B97" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B97" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A100" s="4" t="s">
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>0</v>
+      </c>
+      <c r="B98" s="6">
+        <v>0</v>
+      </c>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+    </row>
+    <row r="101" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A101" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B100" s="4"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B102" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C102" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="E102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F102" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B103" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C103" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D103" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E103" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F103" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B103" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C103" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D103" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E103" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F103" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>0</v>
+      </c>
+      <c r="B104" s="6">
+        <v>0</v>
+      </c>
+      <c r="C104" s="6">
+        <v>0</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0</v>
+      </c>
+      <c r="E104" s="6">
+        <v>0</v>
+      </c>
+      <c r="F104" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B106" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C106" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D106" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E105" s="5" t="s">
+      <c r="E106" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F105" s="5" t="s">
+      <c r="F106" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B107" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C106" s="5" t="s">
+      <c r="C107" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D107" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E106" s="5" t="s">
+      <c r="E107" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F106" s="5" t="s">
+      <c r="F107" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B107" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C107" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D107" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E107" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F107" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="6">
+        <v>0</v>
+      </c>
+      <c r="B108" s="6">
+        <v>0</v>
+      </c>
+      <c r="C108" s="6">
+        <v>0</v>
+      </c>
+      <c r="D108" s="6">
+        <v>0</v>
+      </c>
+      <c r="E108" s="6">
+        <v>0</v>
+      </c>
+      <c r="F108" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B110" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C110" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D110" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E109" s="5" t="s">
+      <c r="E110" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F109" s="5" t="s">
+      <c r="F110" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B111" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="C111" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D111" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E110" s="5" t="s">
+      <c r="E111" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F110" s="5" t="s">
+      <c r="F111" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B111" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="C111" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="D111" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E111" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F111" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="6">
+        <v>0</v>
+      </c>
+      <c r="B112" s="6">
+        <v>0</v>
+      </c>
+      <c r="C112" s="6">
+        <v>0</v>
+      </c>
+      <c r="D112" s="6">
+        <v>0</v>
+      </c>
+      <c r="E112" s="6">
+        <v>0</v>
+      </c>
+      <c r="F112" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B114" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C114" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D114" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B115" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C115" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D115" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B115" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C115" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D115" s="5">
-        <v>0</v>
-      </c>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-    </row>
-    <row r="118" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A118" s="4" t="s">
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="6">
+        <v>0</v>
+      </c>
+      <c r="B116" s="6">
+        <v>0</v>
+      </c>
+      <c r="C116" s="6">
+        <v>0</v>
+      </c>
+      <c r="D116" s="6">
+        <v>0</v>
+      </c>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+    </row>
+    <row r="119" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A119" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B118" s="4"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
+      <c r="B119" s="5"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B120" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C119" s="5" t="s">
+      <c r="C120" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D120" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="5" t="s">
+      <c r="E120" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F119" s="5" t="s">
+      <c r="F120" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="B121" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C120" s="5" t="s">
+      <c r="C121" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D121" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E120" s="5" t="s">
+      <c r="E121" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F120" s="5" t="s">
+      <c r="F121" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B121" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C121" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D121" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E121" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F121" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="6">
+        <v>0</v>
+      </c>
+      <c r="B122" s="6">
+        <v>0</v>
+      </c>
+      <c r="C122" s="6">
+        <v>0</v>
+      </c>
+      <c r="D122" s="6">
+        <v>0</v>
+      </c>
+      <c r="E122" s="6">
+        <v>0</v>
+      </c>
+      <c r="F122" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B124" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C123" s="5" t="s">
+      <c r="C124" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D124" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E123" s="5" t="s">
+      <c r="E124" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F123" s="5" t="s">
+      <c r="F124" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B125" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C124" s="5" t="s">
+      <c r="C125" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D125" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E124" s="5" t="s">
+      <c r="E125" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F124" s="5" t="s">
+      <c r="F125" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B125" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C125" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D125" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E125" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F125" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="6">
+        <v>0</v>
+      </c>
+      <c r="B126" s="6">
+        <v>0</v>
+      </c>
+      <c r="C126" s="6">
+        <v>0</v>
+      </c>
+      <c r="D126" s="6">
+        <v>0</v>
+      </c>
+      <c r="E126" s="6">
+        <v>0</v>
+      </c>
+      <c r="F126" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B128" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C128" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D128" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E127" s="5" t="s">
+      <c r="E128" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F127" s="5" t="s">
+      <c r="F128" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B129" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="C129" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D128" s="5" t="s">
+      <c r="D129" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E128" s="5" t="s">
+      <c r="E129" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F128" s="5" t="s">
+      <c r="F129" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B129" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="C129" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="D129" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E129" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F129" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="6">
+        <v>0</v>
+      </c>
+      <c r="B130" s="6">
+        <v>0</v>
+      </c>
+      <c r="C130" s="6">
+        <v>0</v>
+      </c>
+      <c r="D130" s="6">
+        <v>0</v>
+      </c>
+      <c r="E130" s="6">
+        <v>0</v>
+      </c>
+      <c r="F130" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B132" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C131" s="5" t="s">
+      <c r="C132" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D132" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E131" s="5" t="s">
+      <c r="E132" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F131" s="5" t="s">
+      <c r="F132" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B133" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C132" s="5" t="s">
+      <c r="C133" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D133" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E132" s="5" t="s">
+      <c r="E133" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F132" s="5" t="s">
+      <c r="F133" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B133" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C133" s="5">
-        <v>40.29</v>
-      </c>
-      <c r="D133" s="5">
-        <v>34.15</v>
-      </c>
-      <c r="E133" s="5">
-        <v>0</v>
-      </c>
-      <c r="F133" s="5">
-        <v>34.4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A136" s="4" t="s">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="6">
+        <v>0</v>
+      </c>
+      <c r="B134" s="6">
+        <v>0</v>
+      </c>
+      <c r="C134" s="6">
+        <v>0</v>
+      </c>
+      <c r="D134" s="6">
+        <v>0</v>
+      </c>
+      <c r="E134" s="6">
+        <v>0</v>
+      </c>
+      <c r="F134" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A137" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B136" s="4"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
+      <c r="B137" s="5"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B137" s="5" t="s">
+      <c r="B138" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C137" s="5" t="s">
+      <c r="C138" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D137" s="5" t="s">
+      <c r="D138" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E137" s="5" t="s">
+      <c r="E138" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F137" s="5" t="s">
+      <c r="F138" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B138" s="5" t="s">
+      <c r="B139" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C139" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D138" s="5" t="s">
+      <c r="D139" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E138" s="5" t="s">
+      <c r="E139" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F138" s="5" t="s">
+      <c r="F139" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B139" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C139" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D139" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E139" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F139" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="6">
+        <v>0</v>
+      </c>
+      <c r="B140" s="6">
+        <v>0</v>
+      </c>
+      <c r="C140" s="6">
+        <v>0</v>
+      </c>
+      <c r="D140" s="6">
+        <v>0</v>
+      </c>
+      <c r="E140" s="6">
+        <v>0</v>
+      </c>
+      <c r="F140" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B141" s="5" t="s">
+      <c r="B142" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C141" s="5" t="s">
+      <c r="C142" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D142" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E141" s="5" t="s">
+      <c r="E142" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F141" s="5" t="s">
+      <c r="F142" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B142" s="5" t="s">
+      <c r="B143" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C142" s="5" t="s">
+      <c r="C143" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D142" s="5" t="s">
+      <c r="D143" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E142" s="5" t="s">
+      <c r="E143" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F142" s="5" t="s">
+      <c r="F143" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B143" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C143" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="D143" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E143" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F143" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="6">
+        <v>0</v>
+      </c>
+      <c r="B144" s="6">
+        <v>0</v>
+      </c>
+      <c r="C144" s="6">
+        <v>0</v>
+      </c>
+      <c r="D144" s="6">
+        <v>0</v>
+      </c>
+      <c r="E144" s="6">
+        <v>0</v>
+      </c>
+      <c r="F144" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B146" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C145" s="5" t="s">
+      <c r="C146" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D145" s="5" t="s">
+      <c r="D146" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E145" s="5" t="s">
+      <c r="E146" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F145" s="5" t="s">
+      <c r="F146" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B147" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C147" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D146" s="5" t="s">
+      <c r="D147" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E146" s="5" t="s">
+      <c r="E147" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F146" s="5" t="s">
+      <c r="F147" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B147" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="C147" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="D147" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E147" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="F147" s="5">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="6">
+        <v>0</v>
+      </c>
+      <c r="B148" s="6">
+        <v>0</v>
+      </c>
+      <c r="C148" s="6">
+        <v>0</v>
+      </c>
+      <c r="D148" s="6">
+        <v>0</v>
+      </c>
+      <c r="E148" s="6">
+        <v>0</v>
+      </c>
+      <c r="F148" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B149" s="5" t="s">
+      <c r="B150" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C149" s="5" t="s">
+      <c r="C150" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D149" s="5" t="s">
+      <c r="D150" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E149" s="5" t="s">
+      <c r="E150" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F149" s="5" t="s">
+      <c r="F150" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B151" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C150" s="5" t="s">
+      <c r="C151" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D151" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E150" s="5" t="s">
+      <c r="E151" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F150" s="5" t="s">
+      <c r="F151" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="B151" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="C151" s="5">
-        <v>40.29</v>
-      </c>
-      <c r="D151" s="5">
-        <v>34.15</v>
-      </c>
-      <c r="E151" s="5">
-        <v>0</v>
-      </c>
-      <c r="F151" s="5">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="6">
+        <v>0</v>
+      </c>
+      <c r="B152" s="6">
+        <v>0</v>
+      </c>
+      <c r="C152" s="6">
+        <v>0</v>
+      </c>
+      <c r="D152" s="6">
+        <v>0</v>
+      </c>
+      <c r="E152" s="6">
+        <v>0</v>
+      </c>
+      <c r="F152" s="6">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A31:B31"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:F5">
+  <conditionalFormatting sqref="A6:F6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2577,7 +2585,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11:F11">
+  <conditionalFormatting sqref="A12:F12">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2627,7 +2635,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:F17">
+  <conditionalFormatting sqref="A18:F18">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2677,7 +2685,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:F23">
+  <conditionalFormatting sqref="A24:F24">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2727,7 +2735,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:F27">
+  <conditionalFormatting sqref="A28:F28">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2745,7 +2753,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:F33">
+  <conditionalFormatting sqref="A34:F34">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2795,7 +2803,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:F37">
+  <conditionalFormatting sqref="A38:F38">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -2829,7 +2837,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:F43">
+  <conditionalFormatting sqref="A44:F44">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -2879,7 +2887,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47:F47">
+  <conditionalFormatting sqref="A48:F48">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -2929,7 +2937,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A51:F51">
+  <conditionalFormatting sqref="A52:F52">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -2947,7 +2955,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:F57">
+  <conditionalFormatting sqref="A58:F58">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -2997,7 +3005,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61:F61">
+  <conditionalFormatting sqref="A62:F62">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -3047,7 +3055,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:F65">
+  <conditionalFormatting sqref="A66:F66">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -3065,7 +3073,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:F71">
+  <conditionalFormatting sqref="A72:F72">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -3115,7 +3123,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A75:F75">
+  <conditionalFormatting sqref="A76:F76">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
@@ -3165,7 +3173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A79:F79">
+  <conditionalFormatting sqref="A80:F80">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
@@ -3199,7 +3207,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A85:F85">
+  <conditionalFormatting sqref="A86:F86">
     <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
@@ -3249,7 +3257,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A89:F89">
+  <conditionalFormatting sqref="A90:F90">
     <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
@@ -3299,7 +3307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A93:F93">
+  <conditionalFormatting sqref="A94:F94">
     <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
@@ -3349,7 +3357,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A97:F97">
+  <conditionalFormatting sqref="A98:F98">
     <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
@@ -3367,7 +3375,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:F103">
+  <conditionalFormatting sqref="A104:F104">
     <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
@@ -3377,7 +3385,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:F103">
+  <conditionalFormatting sqref="A104:F104">
     <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min"/>
@@ -3387,7 +3395,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:F103">
+  <conditionalFormatting sqref="A104:F104">
     <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
@@ -3397,7 +3405,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:F103">
+  <conditionalFormatting sqref="A104:F104">
     <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
@@ -3407,7 +3415,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:F103">
+  <conditionalFormatting sqref="A104:F104">
     <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
@@ -3417,7 +3425,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:F103">
+  <conditionalFormatting sqref="A104:F104">
     <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min"/>
@@ -3427,7 +3435,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107:F107">
+  <conditionalFormatting sqref="A108:F108">
     <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
@@ -3437,7 +3445,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107:F107">
+  <conditionalFormatting sqref="A108:F108">
     <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
@@ -3447,7 +3455,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107:F107">
+  <conditionalFormatting sqref="A108:F108">
     <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
@@ -3457,7 +3465,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107:F107">
+  <conditionalFormatting sqref="A108:F108">
     <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
@@ -3467,7 +3475,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107:F107">
+  <conditionalFormatting sqref="A108:F108">
     <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
@@ -3477,7 +3485,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A107:F107">
+  <conditionalFormatting sqref="A108:F108">
     <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
@@ -3487,7 +3495,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:F111">
+  <conditionalFormatting sqref="A112:F112">
     <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="min"/>
@@ -3497,7 +3505,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:F111">
+  <conditionalFormatting sqref="A112:F112">
     <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="min"/>
@@ -3507,7 +3515,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:F111">
+  <conditionalFormatting sqref="A112:F112">
     <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
@@ -3517,7 +3525,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:F111">
+  <conditionalFormatting sqref="A112:F112">
     <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>
@@ -3527,7 +3535,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:F111">
+  <conditionalFormatting sqref="A112:F112">
     <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="min"/>
@@ -3537,7 +3545,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:F111">
+  <conditionalFormatting sqref="A112:F112">
     <cfRule type="colorScale" priority="118">
       <colorScale>
         <cfvo type="min"/>
@@ -3547,7 +3555,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A115:F115">
+  <conditionalFormatting sqref="A116:F116">
     <cfRule type="colorScale" priority="119">
       <colorScale>
         <cfvo type="min"/>
@@ -3557,7 +3565,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A115:F115">
+  <conditionalFormatting sqref="A116:F116">
     <cfRule type="colorScale" priority="120">
       <colorScale>
         <cfvo type="min"/>
@@ -3567,7 +3575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A115:F115">
+  <conditionalFormatting sqref="A116:F116">
     <cfRule type="colorScale" priority="121">
       <colorScale>
         <cfvo type="min"/>
@@ -3577,7 +3585,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A115:F115">
+  <conditionalFormatting sqref="A116:F116">
     <cfRule type="colorScale" priority="122">
       <colorScale>
         <cfvo type="min"/>
@@ -3587,7 +3595,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A121:F121">
+  <conditionalFormatting sqref="A122:F122">
     <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
@@ -3597,7 +3605,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A121:F121">
+  <conditionalFormatting sqref="A122:F122">
     <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min"/>
@@ -3607,7 +3615,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A121:F121">
+  <conditionalFormatting sqref="A122:F122">
     <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
@@ -3617,7 +3625,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A121:F121">
+  <conditionalFormatting sqref="A122:F122">
     <cfRule type="colorScale" priority="126">
       <colorScale>
         <cfvo type="min"/>
@@ -3627,7 +3635,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A121:F121">
+  <conditionalFormatting sqref="A122:F122">
     <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
@@ -3637,7 +3645,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A121:F121">
+  <conditionalFormatting sqref="A122:F122">
     <cfRule type="colorScale" priority="128">
       <colorScale>
         <cfvo type="min"/>
@@ -3647,7 +3655,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:F125">
+  <conditionalFormatting sqref="A126:F126">
     <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
@@ -3657,7 +3665,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:F125">
+  <conditionalFormatting sqref="A126:F126">
     <cfRule type="colorScale" priority="130">
       <colorScale>
         <cfvo type="min"/>
@@ -3667,7 +3675,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:F125">
+  <conditionalFormatting sqref="A126:F126">
     <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="min"/>
@@ -3677,7 +3685,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:F125">
+  <conditionalFormatting sqref="A126:F126">
     <cfRule type="colorScale" priority="132">
       <colorScale>
         <cfvo type="min"/>
@@ -3687,7 +3695,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:F125">
+  <conditionalFormatting sqref="A126:F126">
     <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
@@ -3697,7 +3705,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:F125">
+  <conditionalFormatting sqref="A126:F126">
     <cfRule type="colorScale" priority="134">
       <colorScale>
         <cfvo type="min"/>
@@ -3707,7 +3715,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:F129">
+  <conditionalFormatting sqref="A130:F130">
     <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="min"/>
@@ -3717,7 +3725,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:F129">
+  <conditionalFormatting sqref="A130:F130">
     <cfRule type="colorScale" priority="136">
       <colorScale>
         <cfvo type="min"/>
@@ -3727,7 +3735,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:F129">
+  <conditionalFormatting sqref="A130:F130">
     <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
@@ -3737,7 +3745,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:F129">
+  <conditionalFormatting sqref="A130:F130">
     <cfRule type="colorScale" priority="138">
       <colorScale>
         <cfvo type="min"/>
@@ -3747,7 +3755,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:F129">
+  <conditionalFormatting sqref="A130:F130">
     <cfRule type="colorScale" priority="139">
       <colorScale>
         <cfvo type="min"/>
@@ -3757,7 +3765,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A129:F129">
+  <conditionalFormatting sqref="A130:F130">
     <cfRule type="colorScale" priority="140">
       <colorScale>
         <cfvo type="min"/>
@@ -3767,7 +3775,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A133:F133">
+  <conditionalFormatting sqref="A134:F134">
     <cfRule type="colorScale" priority="141">
       <colorScale>
         <cfvo type="min"/>
@@ -3777,7 +3785,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A133:F133">
+  <conditionalFormatting sqref="A134:F134">
     <cfRule type="colorScale" priority="142">
       <colorScale>
         <cfvo type="min"/>
@@ -3787,7 +3795,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A133:F133">
+  <conditionalFormatting sqref="A134:F134">
     <cfRule type="colorScale" priority="143">
       <colorScale>
         <cfvo type="min"/>
@@ -3797,7 +3805,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A133:F133">
+  <conditionalFormatting sqref="A134:F134">
     <cfRule type="colorScale" priority="144">
       <colorScale>
         <cfvo type="min"/>
@@ -3807,7 +3815,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A133:F133">
+  <conditionalFormatting sqref="A134:F134">
     <cfRule type="colorScale" priority="145">
       <colorScale>
         <cfvo type="min"/>
@@ -3817,7 +3825,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A133:F133">
+  <conditionalFormatting sqref="A134:F134">
     <cfRule type="colorScale" priority="146">
       <colorScale>
         <cfvo type="min"/>
@@ -3827,7 +3835,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A139:F139">
+  <conditionalFormatting sqref="A140:F140">
     <cfRule type="colorScale" priority="147">
       <colorScale>
         <cfvo type="min"/>
@@ -3837,7 +3845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A139:F139">
+  <conditionalFormatting sqref="A140:F140">
     <cfRule type="colorScale" priority="148">
       <colorScale>
         <cfvo type="min"/>
@@ -3847,7 +3855,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A139:F139">
+  <conditionalFormatting sqref="A140:F140">
     <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="min"/>
@@ -3857,7 +3865,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A139:F139">
+  <conditionalFormatting sqref="A140:F140">
     <cfRule type="colorScale" priority="150">
       <colorScale>
         <cfvo type="min"/>
@@ -3867,7 +3875,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A139:F139">
+  <conditionalFormatting sqref="A140:F140">
     <cfRule type="colorScale" priority="151">
       <colorScale>
         <cfvo type="min"/>
@@ -3877,7 +3885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A139:F139">
+  <conditionalFormatting sqref="A140:F140">
     <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
@@ -3887,7 +3895,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A143:F143">
+  <conditionalFormatting sqref="A144:F144">
     <cfRule type="colorScale" priority="153">
       <colorScale>
         <cfvo type="min"/>
@@ -3897,7 +3905,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A143:F143">
+  <conditionalFormatting sqref="A144:F144">
     <cfRule type="colorScale" priority="154">
       <colorScale>
         <cfvo type="min"/>
@@ -3907,7 +3915,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A143:F143">
+  <conditionalFormatting sqref="A144:F144">
     <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
@@ -3917,7 +3925,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A143:F143">
+  <conditionalFormatting sqref="A144:F144">
     <cfRule type="colorScale" priority="156">
       <colorScale>
         <cfvo type="min"/>
@@ -3927,7 +3935,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A143:F143">
+  <conditionalFormatting sqref="A144:F144">
     <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="min"/>
@@ -3937,7 +3945,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A143:F143">
+  <conditionalFormatting sqref="A144:F144">
     <cfRule type="colorScale" priority="158">
       <colorScale>
         <cfvo type="min"/>
@@ -3947,7 +3955,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:F147">
+  <conditionalFormatting sqref="A148:F148">
     <cfRule type="colorScale" priority="159">
       <colorScale>
         <cfvo type="min"/>
@@ -3957,7 +3965,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:F147">
+  <conditionalFormatting sqref="A148:F148">
     <cfRule type="colorScale" priority="160">
       <colorScale>
         <cfvo type="min"/>
@@ -3967,7 +3975,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:F147">
+  <conditionalFormatting sqref="A148:F148">
     <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="min"/>
@@ -3977,7 +3985,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:F147">
+  <conditionalFormatting sqref="A148:F148">
     <cfRule type="colorScale" priority="162">
       <colorScale>
         <cfvo type="min"/>
@@ -3987,7 +3995,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:F147">
+  <conditionalFormatting sqref="A148:F148">
     <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="min"/>
@@ -3997,7 +4005,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A147:F147">
+  <conditionalFormatting sqref="A148:F148">
     <cfRule type="colorScale" priority="164">
       <colorScale>
         <cfvo type="min"/>
@@ -4007,7 +4015,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:F151">
+  <conditionalFormatting sqref="A152:F152">
     <cfRule type="colorScale" priority="165">
       <colorScale>
         <cfvo type="min"/>
@@ -4017,7 +4025,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:F151">
+  <conditionalFormatting sqref="A152:F152">
     <cfRule type="colorScale" priority="166">
       <colorScale>
         <cfvo type="min"/>
@@ -4027,7 +4035,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:F151">
+  <conditionalFormatting sqref="A152:F152">
     <cfRule type="colorScale" priority="167">
       <colorScale>
         <cfvo type="min"/>
@@ -4037,7 +4045,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:F151">
+  <conditionalFormatting sqref="A152:F152">
     <cfRule type="colorScale" priority="168">
       <colorScale>
         <cfvo type="min"/>
@@ -4047,7 +4055,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:F151">
+  <conditionalFormatting sqref="A152:F152">
     <cfRule type="colorScale" priority="169">
       <colorScale>
         <cfvo type="min"/>
@@ -4057,7 +4065,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A151:F151">
+  <conditionalFormatting sqref="A152:F152">
     <cfRule type="colorScale" priority="170">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>